<commit_message>
1.把测试用例数据放入excel管理：新增excel_utils.py，test_data_util.py底层封装 2.测试方法中引用excel的测试数据login_test.py 3.执行所有用例，测试报告的生成，引用HTMLTestReportCN.py 1)runner包（HTMLTestRunner）--run_all_cases.py 2)测试报告中增加截图: base_page.py selenium_base_case.py----TearDown
</commit_message>
<xml_diff>
--- a/element_infos_datas/element_infos.xlsx
+++ b/element_infos_datas/element_infos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\repositories\PO_UI_Test_Framework\element_infos_datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F766FF4-99C6-4B39-B1C7-52EBE0A76921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA5B478-2698-44C8-A5EE-D24E38414E4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8025" yWindow="4410" windowWidth="18075" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -64,10 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>//input[@name="account"]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>//button[@id="submit"]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,10 +108,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>//span[@class="user-name"]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>//li[@data-id="project"]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -709,6 +701,14 @@
   </si>
   <si>
     <t>//nav[@id="subNavbar"]/ul/li/a[@href="/zentao/my-calendar.html"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//ul[@id="userNav"]/li/a/span[@class="user-name"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//input[@name="account"]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1121,19 +1121,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1153,15 +1153,15 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1170,7 +1170,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1178,7 +1178,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1187,18 +1187,18 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
         <v>129</v>
-      </c>
-      <c r="B5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" t="s">
-        <v>131</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>6</v>
@@ -1234,39 +1234,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>125</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1314,123 +1314,123 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
         <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1467,19 +1467,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1487,275 +1487,275 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
         <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" t="s">
         <v>134</v>
       </c>
-      <c r="C17" t="s">
-        <v>136</v>
-      </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1789,19 +1789,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -1809,194 +1809,194 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>139</v>
-      </c>
       <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2036,39 +2036,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2103,39 +2103,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2143,16 +2143,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
         <v>96</v>
-      </c>
-      <c r="D3" t="s">
-        <v>98</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -2160,16 +2160,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -2194,16 +2194,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>85</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -2211,16 +2211,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -2228,16 +2228,16 @@
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
         <v>94</v>
       </c>
-      <c r="B8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" t="s">
-        <v>96</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -2276,39 +2276,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2316,16 +2316,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>114</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>116</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -2333,16 +2333,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -2383,39 +2383,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>108</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>110</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2423,16 +2423,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -2441,21 +2441,21 @@
         <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -2464,7 +2464,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
@@ -2503,39 +2503,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2543,16 +2543,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>3</v>

</xml_diff>